<commit_message>
Update Data.xlsx with new fuel prices
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -559,7 +559,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -610,7 +610,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-04-19</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -664,7 +664,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2936,6 +2936,19 @@
       </c>
       <c r="C174" t="n">
         <v>44.38</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="7" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>45.36</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +2962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5221,6 +5234,19 @@
       </c>
       <c r="C174" t="n">
         <v>46.58</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="7" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>47.56</v>
       </c>
     </row>
   </sheetData>
@@ -5234,7 +5260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7506,6 +7532,19 @@
       </c>
       <c r="C174" t="n">
         <v>45.52</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="7" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>46.5</v>
       </c>
     </row>
   </sheetData>
@@ -7519,7 +7558,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9791,6 +9830,19 @@
       </c>
       <c r="C174" t="n">
         <v>45.81</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="7" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>46.79</v>
       </c>
     </row>
   </sheetData>
@@ -9804,7 +9856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12076,6 +12128,19 @@
       </c>
       <c r="C174" t="n">
         <v>46.53</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="7" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>47.51</v>
       </c>
     </row>
   </sheetData>
@@ -12089,7 +12154,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14361,6 +14426,19 @@
       </c>
       <c r="C174" t="n">
         <v>46.18</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="7" t="n">
+        <v>45770</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Motorin UltraForce</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>47.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>